<commit_message>
carga de usuarios via csv o excel
</commit_message>
<xml_diff>
--- a/plantilla_de_prueba.xlsx
+++ b/plantilla_de_prueba.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">nombre</t>
   </si>
@@ -28,9 +28,6 @@
     <t xml:space="preserve">matricula</t>
   </si>
   <si>
-    <t xml:space="preserve">telefono</t>
-  </si>
-  <si>
     <t xml:space="preserve">email</t>
   </si>
   <si>
@@ -43,9 +40,6 @@
     <t xml:space="preserve">1-11-111</t>
   </si>
   <si>
-    <t xml:space="preserve">809-581-1111</t>
-  </si>
-  <si>
     <t xml:space="preserve">estudiante1@pucmm.edu.do</t>
   </si>
   <si>
@@ -55,9 +49,6 @@
     <t xml:space="preserve">2-22-2222</t>
   </si>
   <si>
-    <t xml:space="preserve">809-581-2222</t>
-  </si>
-  <si>
     <t xml:space="preserve">estudiante2@pucmm.edu.do</t>
   </si>
   <si>
@@ -65,9 +56,6 @@
   </si>
   <si>
     <t xml:space="preserve">3-33-3333</t>
-  </si>
-  <si>
-    <t xml:space="preserve">809-581-3333</t>
   </si>
   <si>
     <t xml:space="preserve">estudiante3@pucmm.edu.do</t>
@@ -85,6 +73,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -106,6 +95,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -176,17 +166,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.63"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.63"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -202,64 +192,52 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="0" t="n">
+      <c r="D2" s="0" t="n">
         <v>123456789</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="0" t="n">
+      <c r="D3" s="0" t="n">
         <v>123456789</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="0" t="n">
         <v>123456789</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" display="estudiante3@pucmm.edu.do"/>
+    <hyperlink ref="C4" r:id="rId1" display="estudiante3@pucmm.edu.do"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>